<commit_message>
docs: update developer documentation
</commit_message>
<xml_diff>
--- a/doc/smarter-codebase.xlsx
+++ b/doc/smarter-codebase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcdaniel/Desktop/gh/smarter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51774159-C768-FF47-B3BC-3F57C1AB5765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB966321-7615-ED4A-A09D-C3BA7496910A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30080" windowHeight="16920" xr2:uid="{5AEBAD83-C729-964D-BE62-C9284A51C02F}"/>
+    <workbookView xWindow="0" yWindow="1120" windowWidth="26760" windowHeight="14840" xr2:uid="{5AEBAD83-C729-964D-BE62-C9284A51C02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,42 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Account</t>
   </si>
   <si>
-    <t>dashboard</t>
-  </si>
-  <si>
-    <t>api</t>
-  </si>
-  <si>
     <t>Plugin</t>
   </si>
   <si>
     <t>Chat</t>
   </si>
   <si>
-    <t>Chatbot</t>
-  </si>
-  <si>
-    <t>common</t>
-  </si>
-  <si>
-    <t>Django apps</t>
-  </si>
-  <si>
-    <t>Customer-facing services</t>
-  </si>
-  <si>
     <t>lib</t>
   </si>
   <si>
-    <t>Code libraries</t>
-  </si>
-  <si>
     <t>Smarter Codebase</t>
+  </si>
+  <si>
+    <t>apt-get system packages</t>
+  </si>
+  <si>
+    <t>NPM Packages</t>
+  </si>
+  <si>
+    <t>Smarter REST API</t>
+  </si>
+  <si>
+    <t>Customer-facing Services</t>
+  </si>
+  <si>
+    <t>Chatapp</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Code Libraries</t>
+  </si>
+  <si>
+    <t>Dashboard Web App</t>
+  </si>
+  <si>
+    <t>PyPi Packages
+(3 million lines)</t>
+  </si>
+  <si>
+    <t>Ubuntu Linux OS
+(28 million lines)</t>
+  </si>
+  <si>
+    <t>Shared Django Apps
+(8 thousand lines)</t>
   </si>
 </sst>
 </file>
@@ -120,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -143,35 +158,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,139 +600,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F14668-0BED-8E49-A2E3-D2706580EEAD}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="3.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="7"/>
-    <col min="10" max="10" width="10.83203125" style="7"/>
-    <col min="12" max="12" width="3.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="3" max="3" width="3.83203125" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="9" width="15.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="F16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="K3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="F20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F10" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F12" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G16" s="3"/>
-    </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="H20" s="3"/>
-    </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="I22" s="3" t="s">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="F24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="I23" s="3"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="I24" s="3"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="26" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="K26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="K27" s="4"/>
-      <c r="M27" s="4"/>
-    </row>
-    <row r="28" spans="8:13" x14ac:dyDescent="0.2">
-      <c r="K28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="F28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="K26:K28"/>
+  <mergeCells count="15">
+    <mergeCell ref="F24:I26"/>
+    <mergeCell ref="F28:I30"/>
+    <mergeCell ref="F20:G22"/>
+    <mergeCell ref="H20:I22"/>
+    <mergeCell ref="B16:D30"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B7:D13"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>